<commit_message>
Spelling and format correction
</commit_message>
<xml_diff>
--- a/Questionnaire.xlsx
+++ b/Questionnaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/mobile/Containers/Data/Application/1E5BBA48-9485-4B24-A149-AFB528B94407/Library/Application Support/Drafts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="8_{2B953FC7-FE5E-2C4E-949E-DFE1D8DC5356}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{068F1D19-FEB6-B943-98AF-50135D2A0DAC}"/>
+  <xr:revisionPtr revIDLastSave="239" documentId="8_{2B953FC7-FE5E-2C4E-949E-DFE1D8DC5356}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{FA053C0A-6255-8C4F-9AE3-FA2AE3A2D2CC}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>Pekerjaan saya adalah:</t>
   </si>
@@ -157,9 +157,6 @@
     <t>Isikan tanda silang (X) pada jawaban yang menurut anda paling sesuai.</t>
   </si>
   <si>
-    <t>Lanjutkan pengisian kuesioner pada halaman selanjutnya.</t>
-  </si>
-  <si>
     <t>Berikan penilaian Anda untuk masing-masing objek dalam tabel berikut. Masing-masing objek dalam tabel tersebut merepresentasikan sebuah minuman teh. Nilai 1 = Sangat Tidak Suka, dan 5 = Sangat Suka. Isikan tanda silang (X) pada kolom yang bersesuaian.</t>
   </si>
   <si>
@@ -173,6 +170,9 @@
   </si>
   <si>
     <t>Saran bagi peneliti (opsional):</t>
+  </si>
+  <si>
+    <t>Lanjutkan pengisian kuesioner pada halaman berikutnya.</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -452,66 +452,36 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -520,6 +490,42 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -838,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFACB234-1E55-AE4C-A7AF-40DC2A2B7AB9}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{0193CB78-E1EE-5222-BA94-1FEE762106F8}">
-      <selection activeCell="A12" sqref="A12:A13"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{0193CB78-E1EE-5222-BA94-1FEE762106F8}">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -855,40 +861,40 @@
       <c r="A1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="25"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="36">
+      <c r="A3" s="46">
         <v>1</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="32"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="19"/>
       <c r="E3" s="20"/>
       <c r="F3" s="5"/>
@@ -897,7 +903,7 @@
       <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="37"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="13" t="s">
         <v>32</v>
       </c>
@@ -912,7 +918,7 @@
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
@@ -925,7 +931,7 @@
       <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="10" t="s">
         <v>2</v>
       </c>
@@ -938,7 +944,7 @@
       <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="10" t="s">
         <v>1</v>
       </c>
@@ -951,7 +957,7 @@
       <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="10" t="s">
         <v>4</v>
       </c>
@@ -964,7 +970,7 @@
       <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="37"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
@@ -977,7 +983,7 @@
       <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="37"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
@@ -993,43 +999,43 @@
       <c r="A11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
+      <c r="B11" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="36"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="46"/>
       <c r="E13" s="1">
         <v>1</v>
       </c>
@@ -1202,41 +1208,41 @@
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="35"/>
+      <c r="B22" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="45"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="49" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="16"/>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="36" t="s">
+      <c r="D23" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="37" t="s">
+      <c r="E23" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="27"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="17"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="36"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="46"/>
       <c r="E24" s="1">
         <v>1</v>
       </c>
@@ -1339,11 +1345,11 @@
       <c r="I29" s="12"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
+      <c r="A30" s="23">
         <v>15</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="48"/>
+      <c r="C30" s="24" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -1356,145 +1362,135 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="44"/>
+      <c r="A31" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="35"/>
     </row>
     <row r="32" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
     </row>
     <row r="33" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="27">
+      <c r="A33" s="29">
         <v>16</v>
       </c>
-      <c r="B33" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="41"/>
+      <c r="B33" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="26"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="37"/>
-      <c r="B34" s="37" t="s">
+      <c r="A34" s="30"/>
+      <c r="B34" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="37"/>
+      <c r="C34" s="30"/>
       <c r="D34" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="41"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="26"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="37"/>
-      <c r="B35" s="37" t="s">
+      <c r="A35" s="30"/>
+      <c r="B35" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="37"/>
+      <c r="C35" s="30"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="41"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="26"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="37"/>
-      <c r="B36" s="37" t="s">
+      <c r="A36" s="30"/>
+      <c r="B36" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="37"/>
+      <c r="C36" s="30"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="41"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="26"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="37"/>
-      <c r="B37" s="37" t="s">
+      <c r="A37" s="30"/>
+      <c r="B37" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="37"/>
+      <c r="C37" s="30"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="41"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="26"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="37"/>
-      <c r="B38" s="37" t="s">
+      <c r="A38" s="30"/>
+      <c r="B38" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="37"/>
+      <c r="C38" s="30"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="42"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="43"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="28"/>
     </row>
     <row r="39" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="47"/>
-      <c r="C39" s="47"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="47"/>
-      <c r="I39" s="48"/>
+      <c r="A39" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="38"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="B32:I32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="A39:I39"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B11:I11"/>
@@ -1510,6 +1506,16 @@
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="E12:I12"/>
     <mergeCell ref="E23:I23"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A39:I39"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Added explanatory text on ID Responden
Clarified that 'ID Responden' would be filled by the researcher, not by
the respondent.
</commit_message>
<xml_diff>
--- a/Questionnaire.xlsx
+++ b/Questionnaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/mobile/Containers/Data/Application/1E5BBA48-9485-4B24-A149-AFB528B94407/Library/Application Support/Drafts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="239" documentId="8_{2B953FC7-FE5E-2C4E-949E-DFE1D8DC5356}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{FA053C0A-6255-8C4F-9AE3-FA2AE3A2D2CC}"/>
+  <xr:revisionPtr revIDLastSave="246" documentId="8_{2B953FC7-FE5E-2C4E-949E-DFE1D8DC5356}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{01B78FD3-0154-DE45-A5A3-5A1DE2B3EA89}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,9 +130,6 @@
     <t>Pekerjaan</t>
   </si>
   <si>
-    <t>ID Responden:</t>
-  </si>
-  <si>
     <t>A-</t>
   </si>
   <si>
@@ -173,6 +170,9 @@
   </si>
   <si>
     <t>Lanjutkan pengisian kuesioner pada halaman berikutnya.</t>
+  </si>
+  <si>
+    <t>ID Responden (diisi oleh peneliti):</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -418,7 +418,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -463,23 +462,47 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -492,41 +515,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -844,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFACB234-1E55-AE4C-A7AF-40DC2A2B7AB9}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{0193CB78-E1EE-5222-BA94-1FEE762106F8}">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{0193CB78-E1EE-5222-BA94-1FEE762106F8}">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -858,56 +851,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+    </row>
+    <row r="2" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41"/>
-    </row>
-    <row r="2" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="46">
+      <c r="A3" s="37">
         <v>1</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="30"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="38"/>
+      <c r="B4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="7"/>
@@ -918,7 +911,7 @@
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="30"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
@@ -931,7 +924,7 @@
       <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="10" t="s">
         <v>2</v>
       </c>
@@ -944,7 +937,7 @@
       <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="10" t="s">
         <v>1</v>
       </c>
@@ -957,7 +950,7 @@
       <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="10" t="s">
         <v>4</v>
       </c>
@@ -970,7 +963,7 @@
       <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
@@ -983,26 +976,26 @@
       <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="30"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="22"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="21"/>
     </row>
     <row r="11" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="42"/>
+      <c r="B11" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="31"/>
       <c r="D11" s="32"/>
       <c r="E11" s="32"/>
       <c r="F11" s="32"/>
@@ -1011,31 +1004,31 @@
       <c r="I11" s="32"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="46"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="37"/>
       <c r="E13" s="1">
         <v>1</v>
       </c>
@@ -1208,41 +1201,41 @@
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="45"/>
+      <c r="B22" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="36"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="47" t="s">
+      <c r="B23" s="15"/>
+      <c r="C23" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="33"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="46"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="37"/>
       <c r="E24" s="1">
         <v>1</v>
       </c>
@@ -1263,8 +1256,8 @@
       <c r="A25" s="10">
         <v>10</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="15" t="s">
+      <c r="B25" s="16"/>
+      <c r="C25" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="10" t="s">
@@ -1280,8 +1273,8 @@
       <c r="A26" s="10">
         <v>11</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="15" t="s">
+      <c r="B26" s="16"/>
+      <c r="C26" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D26" s="10" t="s">
@@ -1297,8 +1290,8 @@
       <c r="A27" s="10">
         <v>12</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="15" t="s">
+      <c r="B27" s="16"/>
+      <c r="C27" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="10" t="s">
@@ -1314,8 +1307,8 @@
       <c r="A28" s="10">
         <v>13</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="15" t="s">
+      <c r="B28" s="16"/>
+      <c r="C28" s="14" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="10" t="s">
@@ -1331,25 +1324,25 @@
       <c r="A29" s="4">
         <v>14</v>
       </c>
-      <c r="B29" s="17"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="6" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="23">
+      <c r="A30" s="22">
         <v>15</v>
       </c>
-      <c r="B30" s="48"/>
-      <c r="C30" s="24" t="s">
+      <c r="B30" s="28"/>
+      <c r="C30" s="23" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -1362,136 +1355,146 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="35"/>
+      <c r="A31" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="42"/>
     </row>
     <row r="32" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
     </row>
     <row r="33" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="29">
+      <c r="A33" s="39">
         <v>16</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C33" s="32"/>
       <c r="D33" s="32"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="26"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="25"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="30"/>
+      <c r="A34" s="38"/>
+      <c r="B34" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="38"/>
       <c r="D34" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="26"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="25"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="30"/>
-      <c r="B35" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="30"/>
+      <c r="A35" s="38"/>
+      <c r="B35" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="38"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="26"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="25"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="30"/>
-      <c r="B36" s="30" t="s">
+      <c r="A36" s="38"/>
+      <c r="B36" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="38"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="25"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="38"/>
+      <c r="B37" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="26"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30" t="s">
+      <c r="C37" s="38"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="25"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="38"/>
+      <c r="B38" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="30"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="26"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="30"/>
+      <c r="C38" s="38"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="28"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="27"/>
     </row>
     <row r="39" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="38"/>
+      <c r="A39" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="44"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="45"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="B1:I1"/>
+  <mergeCells count="26">
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A39:I39"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B2:I2"/>
@@ -1506,16 +1509,7 @@
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="E12:I12"/>
     <mergeCell ref="E23:I23"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="B32:I32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="A39:I39"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Added right arrow to flip to next page and corrected wording
</commit_message>
<xml_diff>
--- a/Questionnaire.xlsx
+++ b/Questionnaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/mobile/Containers/Data/Application/1E5BBA48-9485-4B24-A149-AFB528B94407/Library/Application Support/Drafts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="254" documentId="8_{2B953FC7-FE5E-2C4E-949E-DFE1D8DC5356}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{D69C50D8-EEBF-3345-9B01-2033A1ECE3B5}"/>
+  <xr:revisionPtr revIDLastSave="255" documentId="8_{2B953FC7-FE5E-2C4E-949E-DFE1D8DC5356}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{48A5BD93-2AF5-0946-BEF8-3020E7CDCA88}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>Pekerjaan saya adalah:</t>
   </si>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t>ID Responden (diisi oleh peneliti):</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -467,14 +464,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -491,15 +500,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -517,9 +517,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -840,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFACB234-1E55-AE4C-A7AF-40DC2A2B7AB9}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{0193CB78-E1EE-5222-BA94-1FEE762106F8}">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{0193CB78-E1EE-5222-BA94-1FEE762106F8}">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -854,43 +851,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="46">
+      <c r="A3" s="29">
         <v>1</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="35"/>
+      <c r="C3" s="39"/>
       <c r="D3" s="18"/>
       <c r="E3" s="19"/>
       <c r="F3" s="5"/>
@@ -995,16 +992,16 @@
       <c r="A11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
@@ -1016,7 +1013,7 @@
       <c r="C12" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="38" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="30" t="s">
@@ -1031,7 +1028,7 @@
       <c r="A13" s="31"/>
       <c r="B13" s="31"/>
       <c r="C13" s="31"/>
-      <c r="D13" s="46"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="1">
         <v>1</v>
       </c>
@@ -1062,9 +1059,7 @@
         <v>7000</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1082,9 +1077,7 @@
       <c r="D15" s="2">
         <v>5000</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1107,9 +1100,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -1125,9 +1116,7 @@
         <v>7000</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1146,9 +1135,7 @@
         <v>9000</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1167,9 +1154,7 @@
         <v>9000</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1188,9 +1173,7 @@
         <v>7000</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1208,9 +1191,7 @@
       <c r="D21" s="2">
         <v>11000</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1220,26 +1201,26 @@
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="46"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="41" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="29" t="s">
         <v>21</v>
       </c>
       <c r="E23" s="31" t="s">
@@ -1251,10 +1232,10 @@
       <c r="I23" s="31"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
+      <c r="A24" s="38"/>
       <c r="B24" s="16"/>
       <c r="C24" s="47"/>
-      <c r="D24" s="46"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="1">
         <v>1</v>
       </c>
@@ -1374,42 +1355,42 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="36"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="40"/>
     </row>
     <row r="32" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
     </row>
     <row r="33" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="30">
         <v>16</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
       <c r="E33" s="24"/>
       <c r="F33" s="24"/>
       <c r="G33" s="24"/>
@@ -1484,17 +1465,17 @@
       <c r="I38" s="27"/>
     </row>
     <row r="39" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="38"/>
-      <c r="I39" s="39"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="35"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -1503,6 +1484,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="E12:I12"/>
     <mergeCell ref="E23:I23"/>
@@ -1519,16 +1510,6 @@
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="A31:I31"/>
     <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C23:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>